<commit_message>
Task #50723: Bulk upload sample file changed
</commit_message>
<xml_diff>
--- a/apps/client-assets/assets/common/user-bulk-upload-sample.xlsx
+++ b/apps/client-assets/assets/common/user-bulk-upload-sample.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>firstname</t>
   </si>
@@ -22,19 +22,22 @@
     <t>email</t>
   </si>
   <si>
-    <t>Christopher</t>
+    <t>TestUserFirstName</t>
+  </si>
+  <si>
+    <t>TestUserLastName</t>
+  </si>
+  <si>
+    <t>testuser@test.com</t>
+  </si>
+  <si>
+    <t>Christy</t>
   </si>
   <si>
     <t>Fernandes</t>
   </si>
   <si>
-    <t>christopher@test.com</t>
-  </si>
-  <si>
-    <t>Christy</t>
-  </si>
-  <si>
-    <t>christy@test.com</t>
+    <t>test12email@test.com</t>
   </si>
   <si>
     <t>Test</t>
@@ -43,7 +46,7 @@
     <t>test</t>
   </si>
   <si>
-    <t>test@test.com</t>
+    <t>testemail123@test.com</t>
   </si>
 </sst>
 </file>
@@ -301,6 +304,11 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="32.57"/>
+    <col customWidth="1" min="2" max="2" width="32.29"/>
+    <col customWidth="1" min="3" max="3" width="29.86"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
@@ -314,10 +322,10 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C2" s="1" t="s">
@@ -329,21 +337,21 @@
         <v>6</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="2" t="s">
         <v>7</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="2" t="s">
         <v>10</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Task #51400: New sample file added with roles
</commit_message>
<xml_diff>
--- a/apps/client-assets/assets/common/user-bulk-upload-sample.xlsx
+++ b/apps/client-assets/assets/common/user-bulk-upload-sample.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="19">
   <si>
     <t>firstname</t>
   </si>
@@ -22,15 +22,33 @@
     <t>email</t>
   </si>
   <si>
+    <t>admin</t>
+  </si>
+  <si>
+    <t>reviewer</t>
+  </si>
+  <si>
+    <t>publisher</t>
+  </si>
+  <si>
+    <t>editor</t>
+  </si>
+  <si>
+    <t>content-creator</t>
+  </si>
+  <si>
     <t>TestUserFirstName</t>
   </si>
   <si>
-    <t>TestUserLastName</t>
+    <t>F'des</t>
   </si>
   <si>
     <t>testuser@test.com</t>
   </si>
   <si>
+    <t>Y</t>
+  </si>
+  <si>
     <t>Christy</t>
   </si>
   <si>
@@ -40,10 +58,13 @@
     <t>test12email@test.com</t>
   </si>
   <si>
+    <t>N</t>
+  </si>
+  <si>
     <t>Test</t>
   </si>
   <si>
-    <t>test</t>
+    <t>test's</t>
   </si>
   <si>
     <t>testemail123@test.com</t>
@@ -53,24 +74,34 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
-    <font/>
     <font>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
+    <font/>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="lightGray"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -79,14 +110,17 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -314,45 +348,109 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>5</v>
+        <v>10</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>7</v>
+      <c r="A3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>8</v>
+        <v>14</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>10</v>
+      <c r="A4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>17</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>11</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>